<commit_message>
experiment to find the statistical features
</commit_message>
<xml_diff>
--- a/GasNodes.xlsx
+++ b/GasNodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wany105\OneDrive - Vanderbilt\Research\ShelbyCounty_DataRead\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Infrastructure-network-simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{08209629-FAA1-49D4-8BAC-BED9493AFE4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2981826-D9EA-46A5-89D5-3EA8DAE42D26}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{08209629-FAA1-49D4-8BAC-BED9493AFE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{816CCFE7-BB84-42F2-B993-1ADB046F08C7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8348" yWindow="915" windowWidth="9045" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,19 +45,19 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Gate Station</t>
-  </si>
-  <si>
-    <t>Regulator Station</t>
-  </si>
-  <si>
     <t>Lat</t>
   </si>
   <si>
     <t>Long</t>
+  </si>
+  <si>
+    <t>Gas pumping station</t>
+  </si>
+  <si>
+    <t>Intermediate station</t>
+  </si>
+  <si>
+    <t>Deliver station</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -428,10 +428,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -442,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>742617</v>
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>835852</v>
@@ -488,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2">
         <v>866472</v>
@@ -511,7 +511,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>775403</v>
@@ -534,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>784629</v>
@@ -557,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>824453</v>
@@ -580,7 +580,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>859983</v>
@@ -603,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>852152</v>
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>850515</v>
@@ -649,7 +649,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2">
         <v>724289</v>
@@ -672,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
         <v>846768</v>
@@ -695,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2">
         <v>865488</v>
@@ -718,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2">
         <v>867887</v>
@@ -741,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2">
         <v>852304</v>
@@ -764,7 +764,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
         <v>881141</v>
@@ -787,7 +787,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2">
         <v>848742</v>

</xml_diff>